<commit_message>
update script to batch process
</commit_message>
<xml_diff>
--- a/scripts/files/image-alt.xlsx
+++ b/scripts/files/image-alt.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B154"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -420,31 +420,1223 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>1024px-Admiral_Bobby_Ray_Inman,_official_CIA_photo,_1983.jpeg</v>
+        <v>00002098_0011.jpg</v>
       </c>
       <c r="B3" t="str">
-        <v>a person in a military uniform</v>
+        <v>a group of people standing in a room with a person in a suit</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2023_08_11_110846.jpg</v>
+        <v>00002098_0012.jpg</v>
       </c>
       <c r="B4" t="str">
-        <v>a group of people standing behind a bar</v>
+        <v>a group of people standing next to a large machine</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>3d-bioprinting.jpeg</v>
+        <v>00002390_0001.jpg</v>
       </c>
       <c r="B5" t="str">
+        <v>a group of people working on a project</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>00005705_0023.jpg</v>
+      </c>
+      <c r="B6" t="str">
+        <v>a group of men standing in a field</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>00005967_0003(1).jpg</v>
+      </c>
+      <c r="B7" t="str">
+        <v>a group of people riding bikes on a street</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>00005967_0003.jpg</v>
+      </c>
+      <c r="B8" t="str">
+        <v>a group of people riding bikes on a street</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>00006854_0002.jpg</v>
+      </c>
+      <c r="B9" t="str">
+        <v>a brick building with a broken roof</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>00006955_0005.jpg</v>
+      </c>
+      <c r="B10" t="str">
+        <v>men working in a room</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>00006962_0001.jpg</v>
+      </c>
+      <c r="B11" t="str">
+        <v>a large building with a field in front of it</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>00007000_0009.jpg</v>
+      </c>
+      <c r="B12" t="str">
+        <v>a group of people posing for a photo</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>00007001_0001.jpg (electrical engineers).jpg</v>
+      </c>
+      <c r="B13" t="str">
+        <v>a group of men in uniform</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>00007004_0001(1).jpg</v>
+      </c>
+      <c r="B14" t="str">
+        <v>a group of people in a factory</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>00007004_0001.jpg</v>
+      </c>
+      <c r="B15" t="str">
+        <v>a group of people in a factory</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>00007005_0006.jpg</v>
+      </c>
+      <c r="B16" t="str">
+        <v>a man sitting at a table</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>00008355_001.jpg</v>
+      </c>
+      <c r="B17" t="str">
+        <v>a man pointing at a man in a suit</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>00015013_0001.jpg</v>
+      </c>
+      <c r="B18" t="str">
+        <v>a group of people raising their hands</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>00018323_004.jpg</v>
+      </c>
+      <c r="B19" t="str">
+        <v>a man looking at a man in a suit</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>00018325_004.jpg</v>
+      </c>
+      <c r="B20" t="str">
+        <v>a machine on the counter</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>00019306_001.jpg</v>
+      </c>
+      <c r="B21" t="str">
+        <v>a man wearing glasses</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>00020166_001.jpg</v>
+      </c>
+      <c r="B22" t="str">
+        <v>a man wearing glasses and a suit</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>00021082_004.jpg</v>
+      </c>
+      <c r="B23" t="str">
+        <v>a group of men looking at a camera</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>1024px-Admiral_Bobby_Ray_Inman,_official_CIA_photo,_1983.jpeg</v>
+      </c>
+      <c r="B24" t="str">
+        <v>a person in a military uniform</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>2023_08_11_110846.jpg</v>
+      </c>
+      <c r="B25" t="str">
+        <v>a group of people standing behind a bar</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>3523ScheinmanHydrArm.jpeg</v>
+      </c>
+      <c r="B26" t="str">
+        <v>a man holding a large skeleton</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>3d-bioprinting.jpg</v>
+      </c>
+      <c r="B27" t="str">
         <v>a computer screen with a logo</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>A-CAM-2022SE-138.jpg</v>
+      </c>
+      <c r="B28" t="str">
+        <v>a building with glass walls</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>A-CAM-2022SE-178.jpg</v>
+      </c>
+      <c r="B29" t="str">
+        <v>a person riding a scooter in front of a building</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>AlexandraBoehm_01_Hi-Res_9828.jpg</v>
+      </c>
+      <c r="B30" t="str">
+        <v>a man smiling outside</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>Barbara_Liskov_computer_scientist_2010.jpg</v>
+      </c>
+      <c r="B31" t="str">
+        <v>a close-up of a person smiling</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>Cartoon EWS.jpg</v>
+      </c>
+      <c r="B32" t="str">
+        <v>a group of people sitting at a table</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>Copy of 00007002_0011.jpg (engineering lab exterior).jpg</v>
+      </c>
+      <c r="B33" t="str">
+        <v>a group of people standing next to a plane</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>Copy of 00007204_0003.jpg (Guggehneim Lab).jpg</v>
+      </c>
+      <c r="B34" t="str">
+        <v>a group of people working in a factory</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>Copy of 00012017_005.jpg</v>
+      </c>
+      <c r="B35" t="str">
+        <v>a stone archway with a staircase</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>Copy of 00014490_015 (1).jpg</v>
+      </c>
+      <c r="B36" t="str">
+        <v>a building with trees in front of it</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>Copy of 00014490_015.jpg</v>
+      </c>
+      <c r="B37" t="str">
+        <v>a building with trees in front of it</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>DF-SC-97-01109.jpeg</v>
+      </c>
+      <c r="B38" t="str">
+        <v>a person standing next to a statue</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>Deisseroth_SteveFisch.jpg</v>
+      </c>
+      <c r="B39" t="str">
+        <v>a man playing the drums</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>Fig.1d.jpg</v>
+      </c>
+      <c r="B40" t="str">
+        <v>close-up of hands holding a puzzle</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Francis and Brad-Press Day.jpg</v>
+      </c>
+      <c r="B41" t="str">
+        <v>a couple of men in blue lab coats holding a large piece of fabric</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>Hoover_EmergingTechEvent_11-14-23_PatrickBeaudouin_IMG_0478.jpg</v>
+      </c>
+      <c r="B42" t="str">
+        <v>a few business women talking</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>Hoover_EmergingTechEvent_QE_11-14-23_PatrickBeaudouin_PTB_2163.jpg</v>
+      </c>
+      <c r="B43" t="str">
+        <v>a man and woman sitting in chairs in front of a large crowd</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>Jelena Vuckovic High-Res.jpg</v>
+      </c>
+      <c r="B44" t="str">
+        <v>a man wearing glasses</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>Jennifer Widom_preferred_ High-Res.jpg</v>
+      </c>
+      <c r="B45" t="str">
+        <v>a man smiling for the camera</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>Majumdar.jpeg</v>
+      </c>
+      <c r="B46" t="str">
+        <v>a man standing in front of a building</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>Map_1966.png</v>
+      </c>
+      <c r="B47" t="str">
+        <v>diagram, engineering drawing</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>Owen Garriott_NASA.jpeg</v>
+      </c>
+      <c r="B48" t="str">
+        <v>a man sitting on a machine</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>P8025899_w4032_q10.jpg</v>
+      </c>
+      <c r="B49" t="str">
+        <v>a man folding his arms</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>PC0062_2008-194_AERIALS_01_009.jpg</v>
+      </c>
+      <c r="B50" t="str">
+        <v>an aerial view of a town</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>PC0062_2008-194_SEQ_04_015.jpg</v>
+      </c>
+      <c r="B51" t="str">
+        <v>a building under construction</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>PC0139_Persis_Drell_2014-09-05_2866.jpg</v>
+      </c>
+      <c r="B52" t="str">
+        <v>a man with gray hair</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>PC0141_b07_Timoshenko_0120.jpg</v>
+      </c>
+      <c r="B53" t="str">
+        <v>a person standing in front of a classroom of people</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>PC0141_b10_Engineering_Corner_0511 EWS2.jpg</v>
+      </c>
+      <c r="B54" t="str">
+        <v>text</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>PC0141_b12_Engineering_Corner_0172.jpg</v>
+      </c>
+      <c r="B55" t="str">
+        <v>a group of people playing in a courtyard</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>Poon_microstimulator_w_penny.jpg</v>
+      </c>
+      <c r="B56" t="str">
+        <v>text</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>SA_inst_team-031804-1712w.jpg</v>
+      </c>
+      <c r="B57" t="str">
+        <v>a group of people in blue lab coats standing in front of a yellow machine</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>SC0122_1981-087_b01_f005.jpg</v>
+      </c>
+      <c r="B58" t="str">
+        <v>diagram</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>SC0122_1992-003_b303_X269-007.jpg</v>
+      </c>
+      <c r="B59" t="str">
+        <v>a woman sitting in a chair</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>SC0122_1998-144_b02_Computers_1985_0030.jpg</v>
+      </c>
+      <c r="B60" t="str">
+        <v>a group of people sitting at a table using computers</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>SC0122_s1_b267_f02_0115-01.jpg</v>
+      </c>
+      <c r="B61" t="str">
+        <v>a group of people standing in front of a structure</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>SC0122_s1_b268_f06_1546-11.jpg</v>
+      </c>
+      <c r="B62" t="str">
+        <v>a group of people standing outside a building</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>SC0122_s1_b269_f10_3000-09.jpg</v>
+      </c>
+      <c r="B63" t="str">
+        <v>a group of people standing outside a building</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>SC0122_s1_b269_f13_3354-11.jpg</v>
+      </c>
+      <c r="B64" t="str">
+        <v>a group of people standing next to a large white banner</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>SC0122_s1_b271_f05_6030-09.jpg</v>
+      </c>
+      <c r="B65" t="str">
+        <v>a group of people sitting at a table with boxes</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>SC0122_s1_b278_f01_C076-02.jpg</v>
+      </c>
+      <c r="B66" t="str">
+        <v>a man wearing glasses and a tie</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>SC0122_s1_b278_f04_C388-13.jpg</v>
+      </c>
+      <c r="B67" t="str">
+        <v>a person on a stage</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>SC0122_s1_b278_f09_C832-06.jpg</v>
+      </c>
+      <c r="B68" t="str">
+        <v>a man and a woman working on a machine</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>SC0122_s1_b278_f10_C958-007.jpg</v>
+      </c>
+      <c r="B69" t="str">
+        <v>a group of men standing in front of a computer</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>SC1041_SAIL_CartDeck_2.jpg</v>
+      </c>
+      <c r="B70" t="str">
+        <v>a bicycle parked on a bridge</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>STS047-37-003~large.jpg</v>
+      </c>
+      <c r="B71" t="str">
+        <v>a man in a room with machines</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>SUBB_SD Aerial Garden Court.jpg</v>
+      </c>
+      <c r="B72" t="str">
+        <v>a large building with a red roof</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>Shenoy_MG_6677.jpg</v>
+      </c>
+      <c r="B73" t="str">
+        <v>a person leaning on a wall</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>Stanford_HAI_1381- web.jpg</v>
+      </c>
+      <c r="B74" t="str">
+        <v>a man and woman posing for a picture</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>U7477.jpg</v>
+      </c>
+      <c r="B75" t="str">
+        <v>a couple of men working on a large metal cylinder</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>WelcomeDay_GroupPhotos_9.26.24_01_O5A0256.jpg</v>
+      </c>
+      <c r="B76" t="str">
+        <v>a group of people wearing red shirts</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>aerial-campus-view-2011.jpg</v>
+      </c>
+      <c r="B77" t="str">
+        <v>an aerial view of a town</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>bb752wg6044.jpg</v>
+      </c>
+      <c r="B78" t="str">
+        <v>a group of men in suits</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>br440jc7470.jpg</v>
+      </c>
+      <c r="B79" t="str">
+        <v>a group of people walking around a building</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>central-energy-facility-2015.jpg</v>
+      </c>
+      <c r="B80" t="str">
+        <v>a group of people sitting around a table with a blue and white object</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>ck707sy2214.jpg</v>
+      </c>
+      <c r="B81" t="str">
+        <v>a man in a suit</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>codeinplace.jpg</v>
+      </c>
+      <c r="B82" t="str">
+        <v>Error generating alt text</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>computation corner dedication.jpg</v>
+      </c>
+      <c r="B83" t="str">
+        <v>a group of people standing in a room</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>david-kelley.jpg</v>
+      </c>
+      <c r="B84" t="str">
+        <v>a man in a suit and tie</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>doerr school.jpg</v>
+      </c>
+      <c r="B85" t="str">
+        <v>a person riding a bicycle in front of a building</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>dschoolcohort.jpeg</v>
+      </c>
+      <c r="B86" t="str">
+        <v>a group of people sitting around a table</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>experimental power lines.jpg</v>
+      </c>
+      <c r="B87" t="str">
+        <v>a black and white photo of a pier with a sign and a body of water in the background</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>faculty meeting 1972.jpg</v>
+      </c>
+      <c r="B88" t="str">
+        <v>a group of people sitting around a table</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>flugge-lotz.jpg</v>
+      </c>
+      <c r="B89" t="str">
+        <v>a person writing on a chalkboard</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>fn928pv3867.jpg</v>
+      </c>
+      <c r="B90" t="str">
+        <v>a large factory machinery</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>fred terman 1977.jpg</v>
+      </c>
+      <c r="B91" t="str">
+        <v>a person standing next to a fence</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>fs075wb6787.jpg</v>
+      </c>
+      <c r="B92" t="str">
+        <v>a man wearing glasses</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>fz107qj0976.jpg</v>
+      </c>
+      <c r="B93" t="str">
+        <v>a group of people walking around a building with palm trees</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>ginzton &amp; accelerator.jpg</v>
+      </c>
+      <c r="B94" t="str">
+        <v>a person in a suit</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>ginzton &amp; kaplan.jpg</v>
+      </c>
+      <c r="B95" t="str">
+        <v>a couple of men in suits</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>google gathering 2005.jpeg</v>
+      </c>
+      <c r="B96" t="str">
+        <v>a group of men posing for a photo</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>hanrahan_pat (1).jpg</v>
+      </c>
+      <c r="B97" t="str">
+        <v>a man smiling with his arms crossed</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>hansen &amp; accelerator.jpg</v>
+      </c>
+      <c r="B98" t="str">
+        <v>a person working on a machine</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>harris j ryan.jpg</v>
+      </c>
+      <c r="B99" t="str">
+        <v>a man in a suit standing next to a small structure</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>hewlett &amp; packard.jpg</v>
+      </c>
+      <c r="B100" t="str">
+        <v>a couple of men working on a sound board</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>hewlett center exterior.jpg</v>
+      </c>
+      <c r="B101" t="str">
+        <v>a group of people walking by a building</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>hewlett-packard dedication.jpg</v>
+      </c>
+      <c r="B102" t="str">
+        <v>a group of men standing outside a building</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>high voltage laboratory.jpg</v>
+      </c>
+      <c r="B103" t="str">
+        <v>a person standing next to a person in a suit</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <v>hugh skilling.jpg</v>
+      </c>
+      <c r="B104" t="str">
+        <v>a man in a suit</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <v>james gibbons 1984.jpg</v>
+      </c>
+      <c r="B105" t="str">
+        <v>a man in a suit smiling</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <v>james plummer.jpg</v>
+      </c>
+      <c r="B106" t="str">
+        <v>a man in a suit and tie</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v>jeffrey ullman.jpg</v>
+      </c>
+      <c r="B107" t="str">
+        <v>a man with a beard and mustache</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v>jennifer-widom.jpg</v>
+      </c>
+      <c r="B108" t="str">
+        <v>a person sitting in front of a screen</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v>jh189cy1846.jpg</v>
+      </c>
+      <c r="B109" t="str">
+        <v>a group of men standing in a room with a checkered floor</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <v>john g herriot.jpg</v>
+      </c>
+      <c r="B110" t="str">
+        <v>a man standing next to a machine</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>john hennessy.jpg</v>
+      </c>
+      <c r="B111" t="str">
+        <v>a man in a suit and tie</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v>john mccarthy chess.jpg</v>
+      </c>
+      <c r="B112" t="str">
+        <v>a person sitting at a desk with a board game</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <v>jx362js8604.jpg</v>
+      </c>
+      <c r="B113" t="str">
+        <v>a couple of men posing for the camera</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <v>kenneth arrow.jpg</v>
+      </c>
+      <c r="B114" t="str">
+        <v>a person speaking to a group of people</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v>kn908nr7305.jpg</v>
+      </c>
+      <c r="B115" t="str">
+        <v>a man sitting at a desk</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="str">
+        <v>linear accelerator first section.jpg</v>
+      </c>
+      <c r="B116" t="str">
+        <v>men working in a factory</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="str">
+        <v>linvill &amp; daughter candance.jpg</v>
+      </c>
+      <c r="B117" t="str">
+        <v>a man and a woman looking at a piece of paper</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="str">
+        <v>mae jamison commencement.jpg</v>
+      </c>
+      <c r="B118" t="str">
+        <v>a person in a graduation gown</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="str">
+        <v>mark iii linear accelerator.jpg</v>
+      </c>
+      <c r="B119" t="str">
+        <v>a factory with several machines</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v>martin hellman 1978.jpg</v>
+      </c>
+      <c r="B120" t="str">
+        <v>a man smiling for the camera</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v>mb981vc1736.jpg</v>
+      </c>
+      <c r="B121" t="str">
+        <v>aerial view of a city</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="str">
+        <v>mechanical_engineering_student.jpeg</v>
+      </c>
+      <c r="B122" t="str">
+        <v>a man looking at a phone</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="str">
+        <v>meindl_mitterand_jobs.jpg</v>
+      </c>
+      <c r="B123" t="str">
+        <v>a group of men in suits</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="str">
+        <v>merkle, hellman, &amp; diffie.jpg</v>
+      </c>
+      <c r="B124" t="str">
+        <v>a group of men looking at a paper</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="str">
+        <v>multivators.jpg</v>
+      </c>
+      <c r="B125" t="str">
+        <v>a few mechanical objects</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="str">
+        <v>murray and taber.jpg</v>
+      </c>
+      <c r="B126" t="str">
+        <v>a man standing on a large white object with a boy holding a paper</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="str">
+        <v>nuclear reactor.jpg</v>
+      </c>
+      <c r="B127" t="str">
+        <v>a group of people walking down a staircase</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="str">
+        <v>nz029jf0057.jpg</v>
+      </c>
+      <c r="B128" t="str">
+        <v>a man squatting down</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="str">
+        <v>original Google server.jpg</v>
+      </c>
+      <c r="B129" t="str">
+        <v>a colorful sculpture of a pyramid</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="str">
+        <v>oussama khatib.jpg</v>
+      </c>
+      <c r="B130" t="str">
+        <v>a group of people sitting in chairs</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="str">
+        <v>pars pro toto.jpg</v>
+      </c>
+      <c r="B131" t="str">
+        <v>a courtyard with trees and benches</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="str">
+        <v>pettit_jn566pd7749.jpg</v>
+      </c>
+      <c r="B132" t="str">
+        <v>a man in a suit</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="str">
+        <v>philip-wong-profile EWS.jpg</v>
+      </c>
+      <c r="B133" t="str">
+        <v>a man wearing glasses</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="str">
+        <v>pk304kr0557 EWS.jpg</v>
+      </c>
+      <c r="B134" t="str">
+        <v>a group of men posing for a photo</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="str">
+        <v>railroad car.jpg</v>
+      </c>
+      <c r="B135" t="str">
+        <v>a group of men standing next to a large truck</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="str">
+        <v>rm634fy8400.jpg</v>
+      </c>
+      <c r="B136" t="str">
+        <v>a group of men in suits looking at a machine</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="str">
+        <v>robot demonstration.jpg</v>
+      </c>
+      <c r="B137" t="str">
+        <v>a group of people standing around a robot</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="str">
+        <v>ronald bracewell 1959.jpg</v>
+      </c>
+      <c r="B138" t="str">
+        <v>a man standing in front of a plane</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="str">
+        <v>russ altman.jpg</v>
+      </c>
+      <c r="B139" t="str">
+        <v>a man wearing headphones and speaking into a microphone</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="str">
+        <v>sebastian-thrun.jpg</v>
+      </c>
+      <c r="B140" t="str">
+        <v>a man talking to another man</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="str">
+        <v>stanford solar car.jpg</v>
+      </c>
+      <c r="B141" t="str">
+        <v>a person riding a bicycle next to a race car</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="str">
+        <v>stanley-2005.jpg</v>
+      </c>
+      <c r="B142" t="str">
+        <v>a group of people standing around a car with a logo on it</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="str">
+        <v>students with professor shah.jpeg</v>
+      </c>
+      <c r="B143" t="str">
+        <v>a group of people looking at a piece of paper</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="str">
+        <v>tarpeh_rod searcy.jpg</v>
+      </c>
+      <c r="B144" t="str">
+        <v>a man smiling for the camera</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="str">
+        <v>terman_qm422bp1949 5.57.39 PM.jpg</v>
+      </c>
+      <c r="B145" t="str">
+        <v>a man wearing glasses and a suit</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="str">
+        <v>theodore hoover.jpg</v>
+      </c>
+      <c r="B146" t="str">
+        <v>a man in a suit</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="str">
+        <v>vinton cerf.jpg</v>
+      </c>
+      <c r="B147" t="str">
+        <v>a man holding a pen</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="str">
+        <v>visitors from france.jpg</v>
+      </c>
+      <c r="B148" t="str">
+        <v>a group of people looking at a computer</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="str">
+        <v>vr758kf1949.jpg</v>
+      </c>
+      <c r="B149" t="str">
+        <v>Rambagh Palace over a river</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="str">
+        <v>william durand.jpg</v>
+      </c>
+      <c r="B150" t="str">
+        <v>a man with a beard</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="str">
+        <v>wx455zm5299.jpg</v>
+      </c>
+      <c r="B151" t="str">
+        <v>a building with a staircase</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="str">
+        <v>xx798bb1141.jpg</v>
+      </c>
+      <c r="B152" t="str">
+        <v>a group of men in suits</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="str">
+        <v>zm384pb3271.jpg</v>
+      </c>
+      <c r="B153" t="str">
+        <v>a couple of men standing next to a machine</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="str">
+        <v>zx844pk9013.jpg</v>
+      </c>
+      <c r="B154" t="str">
+        <v>a couple of men talking</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B154"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>